<commit_message>
small fixes on the text and dataset
</commit_message>
<xml_diff>
--- a/vaccination.xlsx
+++ b/vaccination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Can\Desktop\RR Project\covid-report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A80E393-0F2D-4B89-8284-283DCA75CA20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD800FA1-EC60-4C90-B265-B961A2D34478}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2247,7 +2247,7 @@
     <t>https://twitter.com/MoHCCZim/status/1395814192372981760</t>
   </si>
   <si>
-    <t>© 2021 GitHub, Inc.</t>
+    <t>Afghanistan</t>
   </si>
 </sst>
 </file>
@@ -2566,10 +2566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F213"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A213" sqref="A213:XFD213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2600,6 +2600,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>740</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -6814,11 +6817,6 @@
       </c>
       <c r="F212" t="s">
         <v>739</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A213" t="s">
-        <v>740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>